<commit_message>
Little bit of refactor
</commit_message>
<xml_diff>
--- a/ejemplo.xlsx
+++ b/ejemplo.xlsx
@@ -9,7 +9,8 @@
     <sheet name="Resultado_20231024" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Plantilla" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Resultado_202310241" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Resultado" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Resultado_202310242" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Resultado" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -3118,141 +3119,1349 @@
       <c r="D23" s="4" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="n"/>
-      <c r="B24" s="3" t="n"/>
-      <c r="C24" s="3" t="n"/>
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>Decoracion</t>
+        </is>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>06.30</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>Cuadro_Psicodelico.gcode</t>
+        </is>
+      </c>
       <c r="D24" s="3" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="n"/>
-      <c r="B25" s="4" t="n"/>
-      <c r="C25" s="4" t="n"/>
+      <c r="A25" s="4" t="inlineStr">
+        <is>
+          <t>Decoracion</t>
+        </is>
+      </c>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>06.57</t>
+        </is>
+      </c>
+      <c r="C25" s="4" t="inlineStr">
+        <is>
+          <t>Cuadro_Lobo.gcode</t>
+        </is>
+      </c>
       <c r="D25" s="4" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="3" t="n"/>
-      <c r="B26" s="3" t="n"/>
-      <c r="C26" s="3" t="n"/>
+      <c r="A26" s="3" t="inlineStr">
+        <is>
+          <t>Decoracion</t>
+        </is>
+      </c>
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>07.07</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>Cuadro_Optico.gcode</t>
+        </is>
+      </c>
       <c r="D26" s="3" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="n"/>
-      <c r="B27" s="4" t="n"/>
-      <c r="C27" s="4" t="n"/>
+      <c r="A27" s="4" t="inlineStr">
+        <is>
+          <t>Mansiones de la Locura</t>
+        </is>
+      </c>
+      <c r="B27" s="4" t="inlineStr">
+        <is>
+          <t>11.44</t>
+        </is>
+      </c>
+      <c r="C27" s="4" t="inlineStr">
+        <is>
+          <t>MonsterHolder_25_2x.gcode</t>
+        </is>
+      </c>
       <c r="D27" s="4" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="3" t="n"/>
-      <c r="B28" s="3" t="n"/>
-      <c r="C28" s="3" t="n"/>
+      <c r="A28" s="3" t="inlineStr">
+        <is>
+          <t>Mansiones de la Locura</t>
+        </is>
+      </c>
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>00.27</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="inlineStr">
+        <is>
+          <t>Peana_25mm_x1_30mm_x3.gcode</t>
+        </is>
+      </c>
       <c r="D28" s="3" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="n"/>
-      <c r="B29" s="4" t="n"/>
-      <c r="C29" s="4" t="n"/>
+      <c r="A29" s="4" t="inlineStr">
+        <is>
+          <t>Mansiones de la Locura</t>
+        </is>
+      </c>
+      <c r="B29" s="4" t="inlineStr">
+        <is>
+          <t>00.27</t>
+        </is>
+      </c>
+      <c r="C29" s="4" t="inlineStr">
+        <is>
+          <t>Peana_30mm_x4.gcode</t>
+        </is>
+      </c>
       <c r="D29" s="4" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="3" t="n"/>
-      <c r="B30" s="3" t="n"/>
-      <c r="C30" s="3" t="n"/>
+      <c r="A30" s="3" t="inlineStr">
+        <is>
+          <t>Mansiones de la Locura</t>
+        </is>
+      </c>
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>00.28</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="inlineStr">
+        <is>
+          <t>Peana_25mm_x4.gcode</t>
+        </is>
+      </c>
       <c r="D30" s="3" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="n"/>
-      <c r="B31" s="4" t="n"/>
-      <c r="C31" s="4" t="n"/>
+      <c r="A31" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B31" s="4" t="inlineStr">
+        <is>
+          <t>01.23</t>
+        </is>
+      </c>
+      <c r="C31" s="4" t="inlineStr">
+        <is>
+          <t>Cubo_Enfermedad_Tapa.gcode</t>
+        </is>
+      </c>
       <c r="D31" s="4" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="n"/>
-      <c r="B32" s="3" t="n"/>
-      <c r="C32" s="3" t="n"/>
+      <c r="A32" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B32" s="3" t="inlineStr">
+        <is>
+          <t>01.34</t>
+        </is>
+      </c>
+      <c r="C32" s="3" t="inlineStr">
+        <is>
+          <t>Centros_Investigacion_Base.gcode</t>
+        </is>
+      </c>
       <c r="D32" s="3" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="n"/>
-      <c r="B33" s="4" t="n"/>
-      <c r="C33" s="4" t="n"/>
+      <c r="A33" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B33" s="4" t="inlineStr">
+        <is>
+          <t>01.42</t>
+        </is>
+      </c>
+      <c r="C33" s="4" t="inlineStr">
+        <is>
+          <t>Cubo_Enfermedad.gcode</t>
+        </is>
+      </c>
       <c r="D33" s="4" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="3" t="n"/>
-      <c r="B34" s="3" t="n"/>
-      <c r="C34" s="3" t="n"/>
+      <c r="A34" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B34" s="3" t="inlineStr">
+        <is>
+          <t>02.00</t>
+        </is>
+      </c>
+      <c r="C34" s="3" t="inlineStr">
+        <is>
+          <t>Token_Base.gcode</t>
+        </is>
+      </c>
       <c r="D34" s="3" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="4" t="n"/>
-      <c r="B35" s="4" t="n"/>
-      <c r="C35" s="4" t="n"/>
+      <c r="A35" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B35" s="4" t="inlineStr">
+        <is>
+          <t>02.41</t>
+        </is>
+      </c>
+      <c r="C35" s="4" t="inlineStr">
+        <is>
+          <t>Token_Centros_Tapa.gcode</t>
+        </is>
+      </c>
       <c r="D35" s="4" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="3" t="n"/>
-      <c r="B36" s="3" t="n"/>
-      <c r="C36" s="3" t="n"/>
+      <c r="A36" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B36" s="3" t="inlineStr">
+        <is>
+          <t>02.46</t>
+        </is>
+      </c>
+      <c r="C36" s="3" t="inlineStr">
+        <is>
+          <t>Mazo_Jugador_Tapa.gcode</t>
+        </is>
+      </c>
       <c r="D36" s="3" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="n"/>
-      <c r="B37" s="4" t="n"/>
-      <c r="C37" s="4" t="n"/>
+      <c r="A37" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B37" s="4" t="inlineStr">
+        <is>
+          <t>02.47</t>
+        </is>
+      </c>
+      <c r="C37" s="4" t="inlineStr">
+        <is>
+          <t>_Sujeta_Personajes.gcode</t>
+        </is>
+      </c>
       <c r="D37" s="4" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="3" t="n"/>
-      <c r="B38" s="3" t="n"/>
-      <c r="C38" s="3" t="n"/>
+      <c r="A38" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B38" s="3" t="inlineStr">
+        <is>
+          <t>02.48</t>
+        </is>
+      </c>
+      <c r="C38" s="3" t="inlineStr">
+        <is>
+          <t>Mazo_Infeccion_Tapa.gcode</t>
+        </is>
+      </c>
       <c r="D38" s="3" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="4" t="n"/>
-      <c r="B39" s="4" t="n"/>
-      <c r="C39" s="4" t="n"/>
+      <c r="A39" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B39" s="4" t="inlineStr">
+        <is>
+          <t>02.57</t>
+        </is>
+      </c>
+      <c r="C39" s="4" t="inlineStr">
+        <is>
+          <t>Mazo_Jugador_Base.gcode</t>
+        </is>
+      </c>
       <c r="D39" s="4" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="3" t="n"/>
-      <c r="B40" s="3" t="n"/>
-      <c r="C40" s="3" t="n"/>
+      <c r="A40" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B40" s="3" t="inlineStr">
+        <is>
+          <t>03.00</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="inlineStr">
+        <is>
+          <t>Mazo_Infeccion_Base.gcode</t>
+        </is>
+      </c>
       <c r="D40" s="3" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="n"/>
-      <c r="B41" s="4" t="n"/>
-      <c r="C41" s="4" t="n"/>
+      <c r="A41" s="4" t="inlineStr">
+        <is>
+          <t>Quarto</t>
+        </is>
+      </c>
+      <c r="B41" s="4" t="inlineStr">
+        <is>
+          <t>01.32</t>
+        </is>
+      </c>
+      <c r="C41" s="4" t="inlineStr">
+        <is>
+          <t>Quarto_Piezas.gcode</t>
+        </is>
+      </c>
       <c r="D41" s="4" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="3" t="n"/>
-      <c r="B42" s="3" t="n"/>
-      <c r="C42" s="3" t="n"/>
+      <c r="A42" s="3" t="inlineStr">
+        <is>
+          <t>Quarto</t>
+        </is>
+      </c>
+      <c r="B42" s="3" t="inlineStr">
+        <is>
+          <t>02.01</t>
+        </is>
+      </c>
+      <c r="C42" s="3" t="inlineStr">
+        <is>
+          <t>Quarto_Tablero.gcode</t>
+        </is>
+      </c>
       <c r="D42" s="3" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="4" t="n"/>
-      <c r="B43" s="4" t="n"/>
-      <c r="C43" s="4" t="n"/>
+      <c r="A43" s="4" t="inlineStr">
+        <is>
+          <t>Quarto</t>
+        </is>
+      </c>
+      <c r="B43" s="4" t="inlineStr">
+        <is>
+          <t>02.52</t>
+        </is>
+      </c>
+      <c r="C43" s="4" t="inlineStr">
+        <is>
+          <t>Quarto_Caja.gcode</t>
+        </is>
+      </c>
       <c r="D43" s="4" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="3" t="n"/>
-      <c r="B44" s="3" t="n"/>
-      <c r="C44" s="3" t="n"/>
+      <c r="A44" s="3" t="inlineStr">
+        <is>
+          <t>Utensilios_Hogar</t>
+        </is>
+      </c>
+      <c r="B44" s="3" t="inlineStr">
+        <is>
+          <t>00.21</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="inlineStr">
+        <is>
+          <t>Enganche_Cremallera.gcode</t>
+        </is>
+      </c>
       <c r="D44" s="3" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="n"/>
-      <c r="B45" s="4" t="n"/>
-      <c r="C45" s="4" t="n"/>
+      <c r="A45" s="4" t="inlineStr">
+        <is>
+          <t>Utensilios_Hogar</t>
+        </is>
+      </c>
+      <c r="B45" s="4" t="inlineStr">
+        <is>
+          <t>01.10</t>
+        </is>
+      </c>
+      <c r="C45" s="4" t="inlineStr">
+        <is>
+          <t>Rascador.gcode</t>
+        </is>
+      </c>
       <c r="D45" s="4" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="3" t="n"/>
-      <c r="B46" s="3" t="n"/>
-      <c r="C46" s="3" t="n"/>
+      <c r="A46" s="3" t="inlineStr">
+        <is>
+          <t>Utensilios_Hogar</t>
+        </is>
+      </c>
+      <c r="B46" s="3" t="inlineStr">
+        <is>
+          <t>04.44</t>
+        </is>
+      </c>
+      <c r="C46" s="3" t="inlineStr">
+        <is>
+          <t>Mosqueton_Rosca.gcode</t>
+        </is>
+      </c>
+      <c r="D46" s="3" t="n"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="inlineStr">
+        <is>
+          <t>Utensilios_Hogar</t>
+        </is>
+      </c>
+      <c r="B47" s="4" t="inlineStr">
+        <is>
+          <t>04.58</t>
+        </is>
+      </c>
+      <c r="C47" s="4" t="inlineStr">
+        <is>
+          <t>Soporte_Movil_Enchufe.gcode</t>
+        </is>
+      </c>
+      <c r="D47" s="4" t="n"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="inlineStr">
+        <is>
+          <t>Decoracion</t>
+        </is>
+      </c>
+      <c r="B48" s="3" t="inlineStr">
+        <is>
+          <t>06.30</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="inlineStr">
+        <is>
+          <t>Cuadro_Psicodelico.gcode</t>
+        </is>
+      </c>
+      <c r="D48" s="3" t="n"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="4" t="inlineStr">
+        <is>
+          <t>Decoracion</t>
+        </is>
+      </c>
+      <c r="B49" s="4" t="inlineStr">
+        <is>
+          <t>06.57</t>
+        </is>
+      </c>
+      <c r="C49" s="4" t="inlineStr">
+        <is>
+          <t>Cuadro_Lobo.gcode</t>
+        </is>
+      </c>
+      <c r="D49" s="4" t="n"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="inlineStr">
+        <is>
+          <t>Decoracion</t>
+        </is>
+      </c>
+      <c r="B50" s="3" t="inlineStr">
+        <is>
+          <t>07.07</t>
+        </is>
+      </c>
+      <c r="C50" s="3" t="inlineStr">
+        <is>
+          <t>Cuadro_Optico.gcode</t>
+        </is>
+      </c>
+      <c r="D50" s="3" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col width="26.5703125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="10" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="43.42578125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="8" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
+    <col width="9.140625" customWidth="1" style="1" min="5" max="6"/>
+    <col width="9.140625" customWidth="1" style="1" min="7" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Projecto</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Tiempo</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>Mansiones de la Locura</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>11.44</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>MonsterHolder_25_2x.gcode</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>Mansiones de la Locura</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>00.27</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>Peana_25mm_x1_30mm_x3.gcode</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Mansiones de la Locura</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>00.27</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Peana_30mm_x4.gcode</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>Mansiones de la Locura</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>00.28</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>Peana_25mm_x4.gcode</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>01.23</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Cubo_Enfermedad_Tapa.gcode</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>01.34</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>Centros_Investigacion_Base.gcode</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>01.42</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Cubo_Enfermedad.gcode</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>02.00</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>Token_Base.gcode</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>02.41</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Token_Centros_Tapa.gcode</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>02.46</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="inlineStr">
+        <is>
+          <t>Mazo_Jugador_Tapa.gcode</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>02.47</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>_Sujeta_Personajes.gcode</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>02.48</t>
+        </is>
+      </c>
+      <c r="C13" s="4" t="inlineStr">
+        <is>
+          <t>Mazo_Infeccion_Tapa.gcode</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>02.57</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Mazo_Jugador_Base.gcode</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>03.00</t>
+        </is>
+      </c>
+      <c r="C15" s="4" t="inlineStr">
+        <is>
+          <t>Mazo_Infeccion_Base.gcode</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>Quarto</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>01.32</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>Quarto_Piezas.gcode</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="inlineStr">
+        <is>
+          <t>Quarto</t>
+        </is>
+      </c>
+      <c r="B17" s="4" t="inlineStr">
+        <is>
+          <t>02.01</t>
+        </is>
+      </c>
+      <c r="C17" s="4" t="inlineStr">
+        <is>
+          <t>Quarto_Tablero.gcode</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>Quarto</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>02.52</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Quarto_Caja.gcode</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="inlineStr">
+        <is>
+          <t>Utensilios_Hogar</t>
+        </is>
+      </c>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t>00.21</t>
+        </is>
+      </c>
+      <c r="C19" s="4" t="inlineStr">
+        <is>
+          <t>Enganche_Cremallera.gcode</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>Utensilios_Hogar</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>01.10</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Rascador.gcode</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="inlineStr">
+        <is>
+          <t>Utensilios_Hogar</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>04.44</t>
+        </is>
+      </c>
+      <c r="C21" s="4" t="inlineStr">
+        <is>
+          <t>Mosqueton_Rosca.gcode</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>Utensilios_Hogar</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>04.58</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>Soporte_Movil_Enchufe.gcode</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="inlineStr">
+        <is>
+          <t>Decoracion</t>
+        </is>
+      </c>
+      <c r="B23" s="4" t="inlineStr">
+        <is>
+          <t>06.30</t>
+        </is>
+      </c>
+      <c r="C23" s="4" t="inlineStr">
+        <is>
+          <t>Cuadro_Psicodelico.gcode</t>
+        </is>
+      </c>
+      <c r="D23" s="4" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>Decoracion</t>
+        </is>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>06.57</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>Cuadro_Lobo.gcode</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="inlineStr">
+        <is>
+          <t>Decoracion</t>
+        </is>
+      </c>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>07.07</t>
+        </is>
+      </c>
+      <c r="C25" s="4" t="inlineStr">
+        <is>
+          <t>Cuadro_Optico.gcode</t>
+        </is>
+      </c>
+      <c r="D25" s="4" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="inlineStr">
+        <is>
+          <t>Mansiones de la Locura</t>
+        </is>
+      </c>
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>11.44</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>MonsterHolder_25_2x.gcode</t>
+        </is>
+      </c>
+      <c r="D26" s="3" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="inlineStr">
+        <is>
+          <t>Mansiones de la Locura</t>
+        </is>
+      </c>
+      <c r="B27" s="4" t="inlineStr">
+        <is>
+          <t>00.27</t>
+        </is>
+      </c>
+      <c r="C27" s="4" t="inlineStr">
+        <is>
+          <t>Peana_25mm_x1_30mm_x3.gcode</t>
+        </is>
+      </c>
+      <c r="D27" s="4" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="inlineStr">
+        <is>
+          <t>Mansiones de la Locura</t>
+        </is>
+      </c>
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>00.27</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="inlineStr">
+        <is>
+          <t>Peana_30mm_x4.gcode</t>
+        </is>
+      </c>
+      <c r="D28" s="3" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="inlineStr">
+        <is>
+          <t>Mansiones de la Locura</t>
+        </is>
+      </c>
+      <c r="B29" s="4" t="inlineStr">
+        <is>
+          <t>00.28</t>
+        </is>
+      </c>
+      <c r="C29" s="4" t="inlineStr">
+        <is>
+          <t>Peana_25mm_x4.gcode</t>
+        </is>
+      </c>
+      <c r="D29" s="4" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>01.23</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="inlineStr">
+        <is>
+          <t>Cubo_Enfermedad_Tapa.gcode</t>
+        </is>
+      </c>
+      <c r="D30" s="3" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B31" s="4" t="inlineStr">
+        <is>
+          <t>01.34</t>
+        </is>
+      </c>
+      <c r="C31" s="4" t="inlineStr">
+        <is>
+          <t>Centros_Investigacion_Base.gcode</t>
+        </is>
+      </c>
+      <c r="D31" s="4" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B32" s="3" t="inlineStr">
+        <is>
+          <t>01.42</t>
+        </is>
+      </c>
+      <c r="C32" s="3" t="inlineStr">
+        <is>
+          <t>Cubo_Enfermedad.gcode</t>
+        </is>
+      </c>
+      <c r="D32" s="3" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B33" s="4" t="inlineStr">
+        <is>
+          <t>02.00</t>
+        </is>
+      </c>
+      <c r="C33" s="4" t="inlineStr">
+        <is>
+          <t>Token_Base.gcode</t>
+        </is>
+      </c>
+      <c r="D33" s="4" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B34" s="3" t="inlineStr">
+        <is>
+          <t>02.41</t>
+        </is>
+      </c>
+      <c r="C34" s="3" t="inlineStr">
+        <is>
+          <t>Token_Centros_Tapa.gcode</t>
+        </is>
+      </c>
+      <c r="D34" s="3" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B35" s="4" t="inlineStr">
+        <is>
+          <t>02.46</t>
+        </is>
+      </c>
+      <c r="C35" s="4" t="inlineStr">
+        <is>
+          <t>Mazo_Jugador_Tapa.gcode</t>
+        </is>
+      </c>
+      <c r="D35" s="4" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B36" s="3" t="inlineStr">
+        <is>
+          <t>02.47</t>
+        </is>
+      </c>
+      <c r="C36" s="3" t="inlineStr">
+        <is>
+          <t>_Sujeta_Personajes.gcode</t>
+        </is>
+      </c>
+      <c r="D36" s="3" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B37" s="4" t="inlineStr">
+        <is>
+          <t>02.48</t>
+        </is>
+      </c>
+      <c r="C37" s="4" t="inlineStr">
+        <is>
+          <t>Mazo_Infeccion_Tapa.gcode</t>
+        </is>
+      </c>
+      <c r="D37" s="4" t="n"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B38" s="3" t="inlineStr">
+        <is>
+          <t>02.57</t>
+        </is>
+      </c>
+      <c r="C38" s="3" t="inlineStr">
+        <is>
+          <t>Mazo_Jugador_Base.gcode</t>
+        </is>
+      </c>
+      <c r="D38" s="3" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="inlineStr">
+        <is>
+          <t>Pandemic</t>
+        </is>
+      </c>
+      <c r="B39" s="4" t="inlineStr">
+        <is>
+          <t>03.00</t>
+        </is>
+      </c>
+      <c r="C39" s="4" t="inlineStr">
+        <is>
+          <t>Mazo_Infeccion_Base.gcode</t>
+        </is>
+      </c>
+      <c r="D39" s="4" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="inlineStr">
+        <is>
+          <t>Quarto</t>
+        </is>
+      </c>
+      <c r="B40" s="3" t="inlineStr">
+        <is>
+          <t>01.32</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="inlineStr">
+        <is>
+          <t>Quarto_Piezas.gcode</t>
+        </is>
+      </c>
+      <c r="D40" s="3" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="4" t="inlineStr">
+        <is>
+          <t>Quarto</t>
+        </is>
+      </c>
+      <c r="B41" s="4" t="inlineStr">
+        <is>
+          <t>02.01</t>
+        </is>
+      </c>
+      <c r="C41" s="4" t="inlineStr">
+        <is>
+          <t>Quarto_Tablero.gcode</t>
+        </is>
+      </c>
+      <c r="D41" s="4" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="inlineStr">
+        <is>
+          <t>Quarto</t>
+        </is>
+      </c>
+      <c r="B42" s="3" t="inlineStr">
+        <is>
+          <t>02.52</t>
+        </is>
+      </c>
+      <c r="C42" s="3" t="inlineStr">
+        <is>
+          <t>Quarto_Caja.gcode</t>
+        </is>
+      </c>
+      <c r="D42" s="3" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="inlineStr">
+        <is>
+          <t>Utensilios_Hogar</t>
+        </is>
+      </c>
+      <c r="B43" s="4" t="inlineStr">
+        <is>
+          <t>00.21</t>
+        </is>
+      </c>
+      <c r="C43" s="4" t="inlineStr">
+        <is>
+          <t>Enganche_Cremallera.gcode</t>
+        </is>
+      </c>
+      <c r="D43" s="4" t="n"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="inlineStr">
+        <is>
+          <t>Utensilios_Hogar</t>
+        </is>
+      </c>
+      <c r="B44" s="3" t="inlineStr">
+        <is>
+          <t>01.10</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="inlineStr">
+        <is>
+          <t>Rascador.gcode</t>
+        </is>
+      </c>
+      <c r="D44" s="3" t="n"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="inlineStr">
+        <is>
+          <t>Utensilios_Hogar</t>
+        </is>
+      </c>
+      <c r="B45" s="4" t="inlineStr">
+        <is>
+          <t>04.44</t>
+        </is>
+      </c>
+      <c r="C45" s="4" t="inlineStr">
+        <is>
+          <t>Mosqueton_Rosca.gcode</t>
+        </is>
+      </c>
+      <c r="D45" s="4" t="n"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="inlineStr">
+        <is>
+          <t>Utensilios_Hogar</t>
+        </is>
+      </c>
+      <c r="B46" s="3" t="inlineStr">
+        <is>
+          <t>04.58</t>
+        </is>
+      </c>
+      <c r="C46" s="3" t="inlineStr">
+        <is>
+          <t>Soporte_Movil_Enchufe.gcode</t>
+        </is>
+      </c>
       <c r="D46" s="3" t="n"/>
     </row>
     <row r="47">

</xml_diff>